<commit_message>
My local changes before rebase
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raju\Desktop\college_voting_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E31DEDF0-19D8-48CA-818C-C70A59875FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F002ED4B-77CF-4559-B2E6-919933345314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EC0CD84C-F8ED-4503-AB57-8BC25CDF026D}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{EC0CD84C-F8ED-4503-AB57-8BC25CDF026D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="100">
   <si>
     <t>roll_number</t>
   </si>
@@ -190,6 +190,150 @@
   </si>
   <si>
     <t>4th</t>
+  </si>
+  <si>
+    <t>23D31A6601</t>
+  </si>
+  <si>
+    <t>23D31A6602</t>
+  </si>
+  <si>
+    <t>23D31A6603</t>
+  </si>
+  <si>
+    <t>23D31A6604</t>
+  </si>
+  <si>
+    <t>23D31A6605</t>
+  </si>
+  <si>
+    <t>23D31A6606</t>
+  </si>
+  <si>
+    <t>23D31A6607</t>
+  </si>
+  <si>
+    <t>23D31A6608</t>
+  </si>
+  <si>
+    <t>23D31A6609</t>
+  </si>
+  <si>
+    <t>23D31A6610</t>
+  </si>
+  <si>
+    <t>23D31A6611</t>
+  </si>
+  <si>
+    <t>23D31A6612</t>
+  </si>
+  <si>
+    <t>23D31A6613</t>
+  </si>
+  <si>
+    <t>23D31A6614</t>
+  </si>
+  <si>
+    <t>23D31A6615</t>
+  </si>
+  <si>
+    <t>23D31A6616</t>
+  </si>
+  <si>
+    <t>23D31A6617</t>
+  </si>
+  <si>
+    <t>23D31A6618</t>
+  </si>
+  <si>
+    <t>23D31A6619</t>
+  </si>
+  <si>
+    <t>23D31A6620</t>
+  </si>
+  <si>
+    <t>23D31A6621</t>
+  </si>
+  <si>
+    <t>23D31A6622</t>
+  </si>
+  <si>
+    <t>23D31A6623</t>
+  </si>
+  <si>
+    <t>23D31A6624</t>
+  </si>
+  <si>
+    <t>23D31A6625</t>
+  </si>
+  <si>
+    <t>23D31A6626</t>
+  </si>
+  <si>
+    <t>23D31A6627</t>
+  </si>
+  <si>
+    <t>23D31A6628</t>
+  </si>
+  <si>
+    <t>23D31A6629</t>
+  </si>
+  <si>
+    <t>23D31A6630</t>
+  </si>
+  <si>
+    <t>23D31A6631</t>
+  </si>
+  <si>
+    <t>23D31A6632</t>
+  </si>
+  <si>
+    <t>23D31A6633</t>
+  </si>
+  <si>
+    <t>23D31A6634</t>
+  </si>
+  <si>
+    <t>23D31A6635</t>
+  </si>
+  <si>
+    <t>23D31A6636</t>
+  </si>
+  <si>
+    <t>23D31A6637</t>
+  </si>
+  <si>
+    <t>23D31A6638</t>
+  </si>
+  <si>
+    <t>23D31A6639</t>
+  </si>
+  <si>
+    <t>23D31A6640</t>
+  </si>
+  <si>
+    <t>23D31A6641</t>
+  </si>
+  <si>
+    <t>23D31A6642</t>
+  </si>
+  <si>
+    <t>23D31A6643</t>
+  </si>
+  <si>
+    <t>23D31A6644</t>
+  </si>
+  <si>
+    <t>23D31A6645</t>
+  </si>
+  <si>
+    <t>23D31A6646</t>
+  </si>
+  <si>
+    <t>23D31A6647</t>
+  </si>
+  <si>
+    <t>3rd</t>
   </si>
 </sst>
 </file>
@@ -556,18 +700,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122FCF23-34CF-476D-99E0-50642B63ACE3}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53:C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +722,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -589,7 +737,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -600,7 +748,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -611,7 +759,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -622,7 +770,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -633,7 +781,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -644,7 +792,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -655,7 +803,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -666,7 +814,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -677,7 +825,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -688,7 +836,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -699,7 +847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -710,7 +858,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -721,7 +869,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -732,7 +880,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1093,6 +1241,523 @@
       </c>
       <c r="C48" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" t="s">
+        <v>50</v>
+      </c>
+      <c r="C60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" t="s">
+        <v>50</v>
+      </c>
+      <c r="C67" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C69" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" t="s">
+        <v>50</v>
+      </c>
+      <c r="C70" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" t="s">
+        <v>50</v>
+      </c>
+      <c r="C72" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" t="s">
+        <v>50</v>
+      </c>
+      <c r="C73" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" t="s">
+        <v>50</v>
+      </c>
+      <c r="C77" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" t="s">
+        <v>50</v>
+      </c>
+      <c r="C78" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" t="s">
+        <v>50</v>
+      </c>
+      <c r="C79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" t="s">
+        <v>50</v>
+      </c>
+      <c r="C80" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" t="s">
+        <v>50</v>
+      </c>
+      <c r="C81" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" t="s">
+        <v>50</v>
+      </c>
+      <c r="C82" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" t="s">
+        <v>50</v>
+      </c>
+      <c r="C83" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" t="s">
+        <v>50</v>
+      </c>
+      <c r="C84" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C85" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" t="s">
+        <v>50</v>
+      </c>
+      <c r="C86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" t="s">
+        <v>50</v>
+      </c>
+      <c r="C87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" t="s">
+        <v>50</v>
+      </c>
+      <c r="C88" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89" t="s">
+        <v>50</v>
+      </c>
+      <c r="C89" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" t="s">
+        <v>50</v>
+      </c>
+      <c r="C90" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91" t="s">
+        <v>50</v>
+      </c>
+      <c r="C91" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" t="s">
+        <v>50</v>
+      </c>
+      <c r="C92" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" t="s">
+        <v>50</v>
+      </c>
+      <c r="C93" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94" t="s">
+        <v>50</v>
+      </c>
+      <c r="C94" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" t="s">
+        <v>50</v>
+      </c>
+      <c r="C95" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>